<commit_message>
Cria roteiro dos testes completos e inclui gabarito esperado.
</commit_message>
<xml_diff>
--- a/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
+++ b/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas.barcellos\Desktop\Projetos\Controle\projdiario\R\rDOU\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas.barcellos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9195"/>
   </bookViews>
   <sheets>
-    <sheet name="Geral" sheetId="1" r:id="rId1"/>
-    <sheet name="Gabarito" sheetId="2" r:id="rId2"/>
+    <sheet name="Gabarito" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Seção</t>
-  </si>
-  <si>
-    <t>Feito</t>
-  </si>
-  <si>
-    <t>Inicio</t>
-  </si>
-  <si>
-    <t>Fim</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="97">
   <si>
     <t>NR_ATO</t>
   </si>
@@ -132,9 +116,6 @@
     <t>DCS</t>
   </si>
   <si>
-    <t>SIM</t>
-  </si>
-  <si>
     <t>PORTARIA Nº 1.177, DE 25 DE MAIO DE 2017</t>
   </si>
   <si>
@@ -246,7 +227,94 @@
     <t>PORTARIA Nº 71, DE 29 DE MAIO DE 2017</t>
   </si>
   <si>
-    <t>DAS/MAPA</t>
+    <t>INSTRUÇÃO NORMATIVA Nº 28, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>INSTRUÇÃO NORMATIVA Nº 29, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>INSTRUÇÃO NORMATIVA Nº 30, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>INSTRUÇÃO NORMATIVA Nº 31, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>INSTRUÇÃO NORMATIVA Nº 32, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>INSTRUÇÃO NORMATIVA Nº 33, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 157, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 158, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 159, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>SMC/MAPA</t>
+  </si>
+  <si>
+    <t>DECISÃO Nº 70, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>SFA-GO/MAPA</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 165, DE 21 DE JULHO DE 2016</t>
+  </si>
+  <si>
+    <t>SFA-SC/MAPA</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 273, DE 19 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 274, DE 19 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 156, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1927, DE 23 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1930, DE 23 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1931, DE 23 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>INMET/MAPA</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 54, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 92, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 93, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 95, DE 24 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>SFA-BA/MAPA</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.405, DE 19 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.406, DE 19 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>SFA-PA/MAPA</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 101, DE 22 DE AGOSTO DE 2016</t>
   </si>
 </sst>
 </file>
@@ -600,76 +668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>42893</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42893</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,37 +691,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -726,19 +729,19 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>2017</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1">
         <v>42893</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -752,19 +755,19 @@
         <v>1175</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>2017</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1">
         <v>42893</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J3">
         <v>6</v>
@@ -778,19 +781,19 @@
         <v>1176</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>2017</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1">
         <v>42893</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>6</v>
@@ -804,19 +807,19 @@
         <v>1211</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>2017</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1">
         <v>42893</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -830,19 +833,19 @@
         <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1">
         <v>42893</v>
       </c>
       <c r="I6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J6">
         <v>7</v>
@@ -856,19 +859,19 @@
         <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>2017</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1">
         <v>42893</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J7">
         <v>9</v>
@@ -882,19 +885,19 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>2017</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1">
         <v>42893</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J8">
         <v>9</v>
@@ -908,16 +911,19 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>2017</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1">
         <v>42893</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J9">
         <v>9</v>
@@ -931,19 +937,19 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1">
         <v>42893</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J10">
         <v>9</v>
@@ -954,19 +960,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>2017</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1">
         <v>42893</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J11">
         <v>9</v>
@@ -977,19 +983,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G12" s="1">
         <v>42893</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J12">
         <v>9</v>
@@ -1000,19 +1006,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>2017</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1">
         <v>42893</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J13">
         <v>9</v>
@@ -1023,19 +1029,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>2017</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G14" s="1">
         <v>42893</v>
       </c>
       <c r="I14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J14">
         <v>9</v>
@@ -1046,19 +1052,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>2017</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1">
         <v>42893</v>
       </c>
       <c r="I15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J15">
         <v>9</v>
@@ -1072,20 +1078,20 @@
         <v>248</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>2017</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2"/>
       <c r="G16" s="1">
         <v>42893</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J16">
         <v>9</v>
@@ -1099,19 +1105,19 @@
         <v>249</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>2017</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1">
         <v>42893</v>
       </c>
       <c r="I17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J17">
         <v>10</v>
@@ -1125,19 +1131,19 @@
         <v>1177</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>2017</v>
       </c>
       <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1">
+        <v>42893</v>
+      </c>
+      <c r="I18" t="s">
         <v>30</v>
-      </c>
-      <c r="G18" s="1">
-        <v>42893</v>
-      </c>
-      <c r="I18" t="s">
-        <v>36</v>
       </c>
       <c r="J18">
         <v>9</v>
@@ -1151,19 +1157,19 @@
         <v>1213</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>2017</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G19" s="1">
         <v>42893</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J19">
         <v>9</v>
@@ -1174,19 +1180,19 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>2017</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G20" s="1">
         <v>42893</v>
       </c>
       <c r="I20" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J20">
         <v>9</v>
@@ -1200,19 +1206,19 @@
         <v>1200</v>
       </c>
       <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>2017</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="1">
+        <v>42893</v>
+      </c>
+      <c r="I21" t="s">
         <v>31</v>
-      </c>
-      <c r="C21">
-        <v>2017</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="1">
-        <v>42893</v>
-      </c>
-      <c r="I21" t="s">
-        <v>37</v>
       </c>
       <c r="J21">
         <v>9</v>
@@ -1226,19 +1232,19 @@
         <v>1201</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G22" s="1">
         <v>42893</v>
       </c>
       <c r="I22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J22">
         <v>9</v>
@@ -1252,19 +1258,19 @@
         <v>1240</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>2017</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1">
         <v>42893</v>
       </c>
       <c r="I23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J23">
         <v>9</v>
@@ -1278,19 +1284,19 @@
         <v>1218</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>2017</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G24" s="1">
         <v>42893</v>
       </c>
       <c r="I24" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J24">
         <v>9</v>
@@ -1304,19 +1310,19 @@
         <v>1219</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>2017</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G25" s="1">
         <v>42893</v>
       </c>
       <c r="I25" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J25">
         <v>9</v>
@@ -1330,19 +1336,19 @@
         <v>1220</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>2017</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G26" s="1">
         <v>42893</v>
       </c>
       <c r="I26" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J26">
         <v>9</v>
@@ -1356,19 +1362,19 @@
         <v>1221</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>2017</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G27" s="1">
         <v>42893</v>
       </c>
       <c r="I27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J27">
         <v>9</v>
@@ -1382,19 +1388,19 @@
         <v>1248</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>2017</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G28" s="1">
         <v>42893</v>
       </c>
       <c r="I28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J28">
         <v>9</v>
@@ -1408,19 +1414,19 @@
         <v>1249</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <v>2017</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G29" s="1">
         <v>42893</v>
       </c>
       <c r="I29" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J29">
         <v>9</v>
@@ -1434,19 +1440,19 @@
         <v>1242</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>2017</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G30" s="1">
         <v>42893</v>
       </c>
       <c r="I30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J30">
         <v>9</v>
@@ -1460,19 +1466,19 @@
         <v>1252</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>2017</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G31" s="1">
         <v>42893</v>
       </c>
       <c r="I31" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J31">
         <v>10</v>
@@ -1486,19 +1492,19 @@
         <v>1253</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C32">
         <v>2017</v>
       </c>
       <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="1">
+        <v>42893</v>
+      </c>
+      <c r="I32" t="s">
         <v>61</v>
-      </c>
-      <c r="G32" s="1">
-        <v>42893</v>
-      </c>
-      <c r="I32" t="s">
-        <v>67</v>
       </c>
       <c r="J32">
         <v>10</v>
@@ -1512,19 +1518,19 @@
         <v>1254</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C33">
         <v>2017</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G33" s="1">
         <v>42893</v>
       </c>
       <c r="I33" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J33">
         <v>10</v>
@@ -1538,19 +1544,19 @@
         <v>1245</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C34">
         <v>2017</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G34" s="1">
         <v>42893</v>
       </c>
       <c r="I34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J34">
         <v>10</v>
@@ -1564,19 +1570,19 @@
         <v>1246</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C35">
         <v>2017</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G35" s="1">
         <v>42893</v>
       </c>
       <c r="I35" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J35">
         <v>10</v>
@@ -1590,19 +1596,19 @@
         <v>1256</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C36">
         <v>2017</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G36" s="1">
         <v>42893</v>
       </c>
       <c r="I36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J36">
         <v>10</v>
@@ -1616,19 +1622,19 @@
         <v>1268</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C37">
         <v>2017</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G37" s="1">
         <v>42893</v>
       </c>
       <c r="I37" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J37">
         <v>10</v>
@@ -1642,19 +1648,19 @@
         <v>1269</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C38">
         <v>2017</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G38" s="1">
         <v>42893</v>
       </c>
       <c r="I38" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J38">
         <v>10</v>
@@ -1668,19 +1674,19 @@
         <v>1270</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C39">
         <v>2017</v>
       </c>
       <c r="D39" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G39" s="1">
         <v>42893</v>
       </c>
       <c r="I39" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J39">
         <v>10</v>
@@ -1694,19 +1700,19 @@
         <v>1271</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C40">
         <v>2017</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G40" s="1">
         <v>42893</v>
       </c>
       <c r="I40" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J40">
         <v>10</v>
@@ -1720,19 +1726,19 @@
         <v>1272</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C41">
         <v>2017</v>
       </c>
       <c r="D41" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G41" s="1">
         <v>42893</v>
       </c>
       <c r="I41" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J41">
         <v>10</v>
@@ -1746,19 +1752,19 @@
         <v>1273</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C42">
         <v>2017</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G42" s="1">
         <v>42893</v>
       </c>
       <c r="I42" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J42">
         <v>10</v>
@@ -1772,19 +1778,19 @@
         <v>1274</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C43">
         <v>2017</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G43" s="1">
         <v>42893</v>
       </c>
       <c r="I43" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J43">
         <v>10</v>
@@ -1798,19 +1804,19 @@
         <v>1275</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C44">
         <v>2017</v>
       </c>
       <c r="D44" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G44" s="1">
         <v>42893</v>
       </c>
       <c r="I44" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J44">
         <v>10</v>
@@ -1824,19 +1830,19 @@
         <v>1276</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C45">
         <v>2017</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G45" s="1">
         <v>42893</v>
       </c>
       <c r="I45" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J45">
         <v>10</v>
@@ -1847,19 +1853,19 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C46">
         <v>2017</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G46" s="1">
         <v>42893</v>
       </c>
       <c r="I46" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J46">
         <v>10</v>
@@ -1873,19 +1879,19 @@
         <v>1260</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C47">
         <v>2017</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G47" s="1">
         <v>42893</v>
       </c>
       <c r="I47" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J47">
         <v>10</v>
@@ -1899,19 +1905,19 @@
         <v>1266</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C48">
         <v>2017</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G48" s="1">
         <v>42893</v>
       </c>
       <c r="I48" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J48">
         <v>10</v>
@@ -1925,19 +1931,19 @@
         <v>1270</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C49">
         <v>2017</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G49" s="1">
         <v>42893</v>
       </c>
       <c r="I49" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J49">
         <v>10</v>
@@ -1951,19 +1957,19 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C50">
         <v>2017</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G50" s="1">
         <v>42893</v>
       </c>
       <c r="I50" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J50">
         <v>10</v>
@@ -1977,19 +1983,19 @@
         <v>1253</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C51">
         <v>2017</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G51" s="1">
         <v>42893</v>
       </c>
       <c r="I51" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J51">
         <v>10</v>
@@ -2000,24 +2006,648 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C52">
         <v>2017</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G52" s="1">
         <v>42893</v>
       </c>
       <c r="I52" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J52">
         <v>11</v>
       </c>
       <c r="K52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>28</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>2016</v>
+      </c>
+      <c r="D53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I53" t="s">
+        <v>67</v>
+      </c>
+      <c r="J53">
+        <v>6</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>29</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>2016</v>
+      </c>
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I54" t="s">
+        <v>68</v>
+      </c>
+      <c r="J54">
+        <v>8</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>30</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>2016</v>
+      </c>
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I55" t="s">
+        <v>69</v>
+      </c>
+      <c r="J55">
+        <v>11</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>31</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>2016</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I56" t="s">
+        <v>70</v>
+      </c>
+      <c r="J56">
+        <v>13</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>2016</v>
+      </c>
+      <c r="D57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I57" t="s">
+        <v>71</v>
+      </c>
+      <c r="J57">
+        <v>13</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58">
+        <v>2016</v>
+      </c>
+      <c r="D58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I58" t="s">
+        <v>72</v>
+      </c>
+      <c r="J58">
+        <v>18</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>157</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>2016</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I59" t="s">
+        <v>73</v>
+      </c>
+      <c r="J59">
+        <v>27</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>158</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>2016</v>
+      </c>
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I60" t="s">
+        <v>74</v>
+      </c>
+      <c r="J60">
+        <v>27</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>159</v>
+      </c>
+      <c r="B61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>2016</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I61" t="s">
+        <v>75</v>
+      </c>
+      <c r="J61">
+        <v>27</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62">
+        <v>2016</v>
+      </c>
+      <c r="D62" t="s">
+        <v>76</v>
+      </c>
+      <c r="G62" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I62" t="s">
+        <v>77</v>
+      </c>
+      <c r="J62">
+        <v>27</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>165</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63">
+        <v>2016</v>
+      </c>
+      <c r="D63" t="s">
+        <v>78</v>
+      </c>
+      <c r="G63" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I63" t="s">
+        <v>79</v>
+      </c>
+      <c r="J63">
+        <v>27</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>273</v>
+      </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64">
+        <v>2016</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G64" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I64" t="s">
+        <v>81</v>
+      </c>
+      <c r="J64">
+        <v>27</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>274</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65">
+        <v>2016</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="G65" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I65" t="s">
+        <v>82</v>
+      </c>
+      <c r="J65">
+        <v>27</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>156</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66">
+        <v>2016</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I66" t="s">
+        <v>83</v>
+      </c>
+      <c r="J66">
+        <v>4</v>
+      </c>
+      <c r="K66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1927</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67">
+        <v>2016</v>
+      </c>
+      <c r="D67" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I67" t="s">
+        <v>84</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+      <c r="K67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1930</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68">
+        <v>2016</v>
+      </c>
+      <c r="D68" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I68" t="s">
+        <v>85</v>
+      </c>
+      <c r="J68">
+        <v>4</v>
+      </c>
+      <c r="K68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1931</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69">
+        <v>2016</v>
+      </c>
+      <c r="D69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I69" t="s">
+        <v>86</v>
+      </c>
+      <c r="J69">
+        <v>4</v>
+      </c>
+      <c r="K69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>54</v>
+      </c>
+      <c r="B70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70">
+        <v>2016</v>
+      </c>
+      <c r="D70" t="s">
+        <v>87</v>
+      </c>
+      <c r="G70" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I70" t="s">
+        <v>88</v>
+      </c>
+      <c r="J70">
+        <v>5</v>
+      </c>
+      <c r="K70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>92</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71">
+        <v>2016</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I71" t="s">
+        <v>89</v>
+      </c>
+      <c r="J71">
+        <v>5</v>
+      </c>
+      <c r="K71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>93</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72">
+        <v>2016</v>
+      </c>
+      <c r="D72" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I72" t="s">
+        <v>90</v>
+      </c>
+      <c r="J72">
+        <v>5</v>
+      </c>
+      <c r="K72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>95</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73">
+        <v>2016</v>
+      </c>
+      <c r="D73" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I73" t="s">
+        <v>91</v>
+      </c>
+      <c r="J73">
+        <v>5</v>
+      </c>
+      <c r="K73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1405</v>
+      </c>
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74">
+        <v>2016</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="G74" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I74" t="s">
+        <v>93</v>
+      </c>
+      <c r="J74">
+        <v>5</v>
+      </c>
+      <c r="K74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1406</v>
+      </c>
+      <c r="B75" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75">
+        <v>2016</v>
+      </c>
+      <c r="D75" t="s">
+        <v>92</v>
+      </c>
+      <c r="G75" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I75" t="s">
+        <v>94</v>
+      </c>
+      <c r="J75">
+        <v>5</v>
+      </c>
+      <c r="K75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>101</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76">
+        <v>2016</v>
+      </c>
+      <c r="D76" t="s">
+        <v>95</v>
+      </c>
+      <c r="G76" s="1">
+        <v>42607</v>
+      </c>
+      <c r="I76" t="s">
+        <v>96</v>
+      </c>
+      <c r="J76">
+        <v>5</v>
+      </c>
+      <c r="K76">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclui testes para campos de ano da norma, data de promulgação, título da norma e seção do DOU. Pequenos ajustes nas funções de limpar texto e separar portarias multiplas
</commit_message>
<xml_diff>
--- a/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
+++ b/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
@@ -203,27 +203,6 @@
     <t>PORTARIA Nº 1.249, DE 31 DE MAIO DE 2017</t>
   </si>
   <si>
-    <t>PORTARIA Nº 1.242, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1.252, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1.253, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1.254, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1.245, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1.246, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1.256, DE 1 DE JUNHO DE 2017</t>
-  </si>
-  <si>
     <t>PORTARIA Nº 71, DE 29 DE MAIO DE 2017</t>
   </si>
   <si>
@@ -248,9 +227,6 @@
     <t>PORTARIA Nº 157, DE 24 DE AGOSTO DE 2016</t>
   </si>
   <si>
-    <t>PORTARIA Nº 158, DE 24 DE AGOSTO DE 2016</t>
-  </si>
-  <si>
     <t>PORTARIA Nº 159, DE 24 DE AGOSTO DE 2016</t>
   </si>
   <si>
@@ -278,15 +254,6 @@
     <t>PORTARIA Nº 156, DE 24 DE AGOSTO DE 2016</t>
   </si>
   <si>
-    <t>PORTARIA Nº 1927, DE 23 DE AGOSTO DE 2016</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1930, DE 23 DE AGOSTO DE 2016</t>
-  </si>
-  <si>
-    <t>PORTARIA Nº 1931, DE 23 DE AGOSTO DE 2016</t>
-  </si>
-  <si>
     <t>PORTARIA Nº 54, DE 24 DE AGOSTO DE 2016</t>
   </si>
   <si>
@@ -317,7 +284,40 @@
     <t>INMET</t>
   </si>
   <si>
-    <t>INSTRUÇÃO NORMATIVA Nº , DE DE 2017</t>
+    <t>INSTRUÇÃO NORMATIVA Nº , DE DE 2017.</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.931, DE 23 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.930, DE 23 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.927, DE 23 DE AGOSTO DE 2016</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.242, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.245, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.246, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.256, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.252, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.253, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 1.254, DE 1º DE JUNHO DE 2017</t>
+  </si>
+  <si>
+    <t>PORTARIA Nº 158, DE 24 DE AGOSTO DE 2016.</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,7 @@
         <v>42893</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="J6">
         <v>7</v>
@@ -871,7 +871,7 @@
         <v>42893</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="J7">
         <v>9</v>
@@ -1478,7 +1478,7 @@
         <v>42893</v>
       </c>
       <c r="I31" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="J31">
         <v>9</v>
@@ -1504,7 +1504,7 @@
         <v>42893</v>
       </c>
       <c r="I32" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="J32">
         <v>10</v>
@@ -1530,7 +1530,7 @@
         <v>42893</v>
       </c>
       <c r="I33" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="J33">
         <v>10</v>
@@ -1556,7 +1556,7 @@
         <v>42893</v>
       </c>
       <c r="I34" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="J34">
         <v>10</v>
@@ -1582,7 +1582,7 @@
         <v>42893</v>
       </c>
       <c r="I35" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="J35">
         <v>10</v>
@@ -1608,7 +1608,7 @@
         <v>42893</v>
       </c>
       <c r="I36" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="J36">
         <v>10</v>
@@ -1634,7 +1634,7 @@
         <v>42893</v>
       </c>
       <c r="I37" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="J37">
         <v>10</v>
@@ -2070,7 +2070,7 @@
         <v>42607</v>
       </c>
       <c r="I54" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="J54">
         <v>6</v>
@@ -2096,7 +2096,7 @@
         <v>42607</v>
       </c>
       <c r="I55" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J55">
         <v>8</v>
@@ -2122,7 +2122,7 @@
         <v>42607</v>
       </c>
       <c r="I56" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J56">
         <v>11</v>
@@ -2148,7 +2148,7 @@
         <v>42607</v>
       </c>
       <c r="I57" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J57">
         <v>13</v>
@@ -2174,7 +2174,7 @@
         <v>42607</v>
       </c>
       <c r="I58" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="J58">
         <v>13</v>
@@ -2200,7 +2200,7 @@
         <v>42607</v>
       </c>
       <c r="I59" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J59">
         <v>18</v>
@@ -2226,7 +2226,7 @@
         <v>42607</v>
       </c>
       <c r="I60" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J60">
         <v>27</v>
@@ -2252,7 +2252,7 @@
         <v>42607</v>
       </c>
       <c r="I61" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="J61">
         <v>27</v>
@@ -2278,7 +2278,7 @@
         <v>42607</v>
       </c>
       <c r="I62" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J62">
         <v>27</v>
@@ -2298,13 +2298,13 @@
         <v>2016</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G63" s="1">
         <v>42607</v>
       </c>
       <c r="I63" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="J63">
         <v>27</v>
@@ -2324,13 +2324,13 @@
         <v>2016</v>
       </c>
       <c r="D64" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G64" s="1">
         <v>42607</v>
       </c>
       <c r="I64" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="J64">
         <v>27</v>
@@ -2350,13 +2350,13 @@
         <v>2016</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G65" s="1">
         <v>42607</v>
       </c>
       <c r="I65" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J65">
         <v>27</v>
@@ -2376,13 +2376,13 @@
         <v>2016</v>
       </c>
       <c r="D66" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G66" s="1">
         <v>42607</v>
       </c>
       <c r="I66" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="J66">
         <v>27</v>
@@ -2408,7 +2408,7 @@
         <v>42607</v>
       </c>
       <c r="I67" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J67">
         <v>4</v>
@@ -2434,7 +2434,7 @@
         <v>42607</v>
       </c>
       <c r="I68" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J68">
         <v>4</v>
@@ -2460,7 +2460,7 @@
         <v>42607</v>
       </c>
       <c r="I69" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J69">
         <v>4</v>
@@ -2486,7 +2486,7 @@
         <v>42607</v>
       </c>
       <c r="I70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J70">
         <v>4</v>
@@ -2506,13 +2506,13 @@
         <v>2016</v>
       </c>
       <c r="D71" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G71" s="1">
         <v>42607</v>
       </c>
       <c r="I71" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J71">
         <v>5</v>
@@ -2538,7 +2538,7 @@
         <v>42607</v>
       </c>
       <c r="I72" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="J72">
         <v>5</v>
@@ -2564,7 +2564,7 @@
         <v>42607</v>
       </c>
       <c r="I73" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="J73">
         <v>5</v>
@@ -2590,7 +2590,7 @@
         <v>42607</v>
       </c>
       <c r="I74" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="J74">
         <v>5</v>
@@ -2610,13 +2610,13 @@
         <v>2016</v>
       </c>
       <c r="D75" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G75" s="1">
         <v>42607</v>
       </c>
       <c r="I75" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="J75">
         <v>5</v>
@@ -2636,13 +2636,13 @@
         <v>2016</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G76" s="1">
         <v>42607</v>
       </c>
       <c r="I76" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J76">
         <v>5</v>
@@ -2662,13 +2662,13 @@
         <v>2016</v>
       </c>
       <c r="D77" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G77" s="1">
         <v>42607</v>
       </c>
       <c r="I77" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="J77">
         <v>5</v>

</xml_diff>

<commit_message>
Alterações para corrigir número da página buscada. i) Não repete informações da páginas para normas individualizadas e ii) muda função de pegar página. iii) Corrige erro no gabarito
</commit_message>
<xml_diff>
--- a/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
+++ b/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
@@ -674,8 +674,8 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
         <v>86</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K7">
         <v>1</v>

</xml_diff>

<commit_message>
Corrige teste e função de tipo para adequar a sigla correta do sistema
</commit_message>
<xml_diff>
--- a/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
+++ b/R/rDOU/tests/testthat/exemplos/completo/gabarito.xlsx
@@ -110,9 +110,6 @@
     <t>ATO</t>
   </si>
   <si>
-    <t>RET</t>
-  </si>
-  <si>
     <t>DCS</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>PORTARIA Nº 158, DE 24 DE AGOSTO DE 2016.</t>
+  </si>
+  <si>
+    <t>ART</t>
   </si>
 </sst>
 </file>
@@ -675,7 +675,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,7 @@
         <v>42893</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J6">
         <v>7</v>
@@ -871,7 +871,7 @@
         <v>42893</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J7">
         <v>7</v>
@@ -911,7 +911,7 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>2017</v>
@@ -937,7 +937,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>2017</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C12">
         <v>2017</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C13">
         <v>2017</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C14">
         <v>2017</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>2017</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C16">
         <v>2017</v>
@@ -1169,7 +1169,7 @@
         <v>42893</v>
       </c>
       <c r="I19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19">
         <v>9</v>
@@ -1195,7 +1195,7 @@
         <v>42893</v>
       </c>
       <c r="I20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J20">
         <v>9</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C21">
         <v>2017</v>
@@ -1238,13 +1238,13 @@
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" s="1">
         <v>42893</v>
       </c>
       <c r="I22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22">
         <v>9</v>
@@ -1264,13 +1264,13 @@
         <v>2017</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G23" s="1">
         <v>42893</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J23">
         <v>9</v>
@@ -1290,13 +1290,13 @@
         <v>2017</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" s="1">
         <v>42893</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J24">
         <v>9</v>
@@ -1316,13 +1316,13 @@
         <v>2017</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G25" s="1">
         <v>42893</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25">
         <v>9</v>
@@ -1342,13 +1342,13 @@
         <v>2017</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" s="1">
         <v>42893</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J26">
         <v>9</v>
@@ -1368,13 +1368,13 @@
         <v>2017</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G27" s="1">
         <v>42893</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J27">
         <v>9</v>
@@ -1394,13 +1394,13 @@
         <v>2017</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G28" s="1">
         <v>42893</v>
       </c>
       <c r="I28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J28">
         <v>9</v>
@@ -1420,13 +1420,13 @@
         <v>2017</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G29" s="1">
         <v>42893</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J29">
         <v>9</v>
@@ -1446,13 +1446,13 @@
         <v>2017</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G30" s="1">
         <v>42893</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J30">
         <v>9</v>
@@ -1472,13 +1472,13 @@
         <v>2017</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G31" s="1">
         <v>42893</v>
       </c>
       <c r="I31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J31">
         <v>9</v>
@@ -1498,13 +1498,13 @@
         <v>2017</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G32" s="1">
         <v>42893</v>
       </c>
       <c r="I32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J32">
         <v>10</v>
@@ -1524,13 +1524,13 @@
         <v>2017</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" s="1">
         <v>42893</v>
       </c>
       <c r="I33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J33">
         <v>10</v>
@@ -1550,13 +1550,13 @@
         <v>2017</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" s="1">
         <v>42893</v>
       </c>
       <c r="I34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J34">
         <v>10</v>
@@ -1576,13 +1576,13 @@
         <v>2017</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G35" s="1">
         <v>42893</v>
       </c>
       <c r="I35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J35">
         <v>10</v>
@@ -1602,13 +1602,13 @@
         <v>2017</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G36" s="1">
         <v>42893</v>
       </c>
       <c r="I36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J36">
         <v>10</v>
@@ -1628,13 +1628,13 @@
         <v>2017</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" s="1">
         <v>42893</v>
       </c>
       <c r="I37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J37">
         <v>10</v>
@@ -1654,13 +1654,13 @@
         <v>2017</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G38" s="1">
         <v>42893</v>
       </c>
       <c r="I38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J38">
         <v>10</v>
@@ -1680,13 +1680,13 @@
         <v>2017</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G39" s="1">
         <v>42893</v>
       </c>
       <c r="I39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J39">
         <v>10</v>
@@ -1706,13 +1706,13 @@
         <v>2017</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G40" s="1">
         <v>42893</v>
       </c>
       <c r="I40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J40">
         <v>10</v>
@@ -1732,13 +1732,13 @@
         <v>2017</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G41" s="1">
         <v>42893</v>
       </c>
       <c r="I41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J41">
         <v>10</v>
@@ -1758,13 +1758,13 @@
         <v>2017</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G42" s="1">
         <v>42893</v>
       </c>
       <c r="I42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J42">
         <v>10</v>
@@ -1784,13 +1784,13 @@
         <v>2017</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G43" s="1">
         <v>42893</v>
       </c>
       <c r="I43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J43">
         <v>10</v>
@@ -1810,13 +1810,13 @@
         <v>2017</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G44" s="1">
         <v>42893</v>
       </c>
       <c r="I44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J44">
         <v>10</v>
@@ -1836,13 +1836,13 @@
         <v>2017</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G45" s="1">
         <v>42893</v>
       </c>
       <c r="I45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J45">
         <v>10</v>
@@ -1862,13 +1862,13 @@
         <v>2017</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G46" s="1">
         <v>42893</v>
       </c>
       <c r="I46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J46">
         <v>10</v>
@@ -1879,13 +1879,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C47">
         <v>2017</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G47" s="1">
         <v>42893</v>
@@ -1911,13 +1911,13 @@
         <v>2017</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G48" s="1">
         <v>42893</v>
       </c>
       <c r="I48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J48">
         <v>10</v>
@@ -1937,13 +1937,13 @@
         <v>2017</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G49" s="1">
         <v>42893</v>
       </c>
       <c r="I49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J49">
         <v>10</v>
@@ -1963,13 +1963,13 @@
         <v>2017</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G50" s="1">
         <v>42893</v>
       </c>
       <c r="I50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J50">
         <v>10</v>
@@ -1989,13 +1989,13 @@
         <v>2017</v>
       </c>
       <c r="D51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G51" s="1">
         <v>42893</v>
       </c>
       <c r="I51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J51">
         <v>10</v>
@@ -2015,13 +2015,13 @@
         <v>2017</v>
       </c>
       <c r="D52" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52" s="1">
+        <v>42893</v>
+      </c>
+      <c r="I52" t="s">
         <v>53</v>
-      </c>
-      <c r="G52" s="1">
-        <v>42893</v>
-      </c>
-      <c r="I52" t="s">
-        <v>54</v>
       </c>
       <c r="J52">
         <v>10</v>
@@ -2032,13 +2032,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C53">
         <v>2017</v>
       </c>
       <c r="D53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G53" s="1">
         <v>42893</v>
@@ -2070,7 +2070,7 @@
         <v>42607</v>
       </c>
       <c r="I54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J54">
         <v>6</v>
@@ -2096,7 +2096,7 @@
         <v>42607</v>
       </c>
       <c r="I55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J55">
         <v>8</v>
@@ -2122,7 +2122,7 @@
         <v>42607</v>
       </c>
       <c r="I56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J56">
         <v>11</v>
@@ -2148,7 +2148,7 @@
         <v>42607</v>
       </c>
       <c r="I57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J57">
         <v>13</v>
@@ -2174,7 +2174,7 @@
         <v>42607</v>
       </c>
       <c r="I58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J58">
         <v>13</v>
@@ -2200,7 +2200,7 @@
         <v>42607</v>
       </c>
       <c r="I59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J59">
         <v>18</v>
@@ -2226,7 +2226,7 @@
         <v>42607</v>
       </c>
       <c r="I60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J60">
         <v>27</v>
@@ -2252,7 +2252,7 @@
         <v>42607</v>
       </c>
       <c r="I61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J61">
         <v>27</v>
@@ -2278,7 +2278,7 @@
         <v>42607</v>
       </c>
       <c r="I62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J62">
         <v>27</v>
@@ -2292,19 +2292,19 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C63">
         <v>2016</v>
       </c>
       <c r="D63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G63" s="1">
         <v>42607</v>
       </c>
       <c r="I63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J63">
         <v>27</v>
@@ -2324,13 +2324,13 @@
         <v>2016</v>
       </c>
       <c r="D64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G64" s="1">
         <v>42607</v>
       </c>
       <c r="I64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J64">
         <v>27</v>
@@ -2350,13 +2350,13 @@
         <v>2016</v>
       </c>
       <c r="D65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G65" s="1">
         <v>42607</v>
       </c>
       <c r="I65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J65">
         <v>27</v>
@@ -2376,13 +2376,13 @@
         <v>2016</v>
       </c>
       <c r="D66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G66" s="1">
         <v>42607</v>
       </c>
       <c r="I66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J66">
         <v>27</v>
@@ -2408,7 +2408,7 @@
         <v>42607</v>
       </c>
       <c r="I67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J67">
         <v>4</v>
@@ -2428,13 +2428,13 @@
         <v>2016</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G68" s="1">
         <v>42607</v>
       </c>
       <c r="I68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J68">
         <v>4</v>
@@ -2454,13 +2454,13 @@
         <v>2016</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G69" s="1">
         <v>42607</v>
       </c>
       <c r="I69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J69">
         <v>4</v>
@@ -2480,13 +2480,13 @@
         <v>2016</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G70" s="1">
         <v>42607</v>
       </c>
       <c r="I70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J70">
         <v>4</v>
@@ -2506,13 +2506,13 @@
         <v>2016</v>
       </c>
       <c r="D71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G71" s="1">
         <v>42607</v>
       </c>
       <c r="I71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J71">
         <v>5</v>
@@ -2538,7 +2538,7 @@
         <v>42607</v>
       </c>
       <c r="I72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J72">
         <v>5</v>
@@ -2564,7 +2564,7 @@
         <v>42607</v>
       </c>
       <c r="I73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J73">
         <v>5</v>
@@ -2590,7 +2590,7 @@
         <v>42607</v>
       </c>
       <c r="I74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J74">
         <v>5</v>
@@ -2610,13 +2610,13 @@
         <v>2016</v>
       </c>
       <c r="D75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G75" s="1">
         <v>42607</v>
       </c>
       <c r="I75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J75">
         <v>5</v>
@@ -2636,13 +2636,13 @@
         <v>2016</v>
       </c>
       <c r="D76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G76" s="1">
         <v>42607</v>
       </c>
       <c r="I76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J76">
         <v>5</v>
@@ -2662,13 +2662,13 @@
         <v>2016</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G77" s="1">
         <v>42607</v>
       </c>
       <c r="I77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J77">
         <v>5</v>

</xml_diff>